<commit_message>
ci: Enable LFS for checkout to fix unit tests
Updates the GitHub Actions workflow to enable Git LFS on checkout.
The unit tests were failing because the test data, which is stored in Git LFS, was not being checked out in the CI environment. Setting `lfs: true` for the `actions/checkout` step resolves this issue.
</commit_message>
<xml_diff>
--- a/data/write_test.xlsx
+++ b/data/write_test.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <workbookPr/>
   <sheets>
-    <sheet name="シート1" r:id="rId4" state="visible" sheetId="1"/>
+    <sheet name="シート1" sheetId="1" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -40,18 +40,18 @@
     <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyFont="1" borderId="0" fontId="0" fillId="0" numFmtId="0" applyAlignment="1"/>
+    <xf numFmtId="0" applyFont="1" borderId="0" fontId="0" applyAlignment="1" fillId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf fontId="0" borderId="0" fillId="0" applyAlignment="1" applyFont="1" numFmtId="0" xfId="0">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fontId="1" applyFont="1" fillId="0" xfId="0" numFmtId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" xfId="0" applyAlignment="1" borderId="0" fillId="0" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" xfId="0" name="Normal"/>
+    <cellStyle name="Normal" builtinId="0" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -142,7 +142,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="0" ang="5400000"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -168,25 +168,25 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="0" ang="5400000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cap="flat" w="6350" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" w="6350" cmpd="sng" cap="flat">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" w="12700" cmpd="sng">
+        <a:ln algn="ctr" w="12700" cap="flat" cmpd="sng">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln cmpd="sng" algn="ctr" w="19050" cap="flat">
+        <a:ln w="19050" algn="ctr" cap="flat" cmpd="sng">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -203,7 +203,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" dist="19050" dir="5400000" blurRad="57150" rotWithShape="0">
+            <a:outerShdw dist="19050" algn="ctr" dir="5400000" blurRad="57150" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -255,9 +255,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+<worksheet xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <sheetPr>
-    <outlinePr summaryRight="0" summaryBelow="0"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -273,10 +273,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c s="1" r="A2">
         <v>2.0</v>
       </c>
-      <c r="B2" s="1">
+      <c s="1" r="B2">
         <v>4.0</v>
       </c>
     </row>

</xml_diff>